<commit_message>
Entregable 10 - exporting updates
</commit_message>
<xml_diff>
--- a/exportaciones/resultados.xlsx
+++ b/exportaciones/resultados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,227 +436,132 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>first_name</t>
+          <t>puntuacion</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>last_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>match_query</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>match_result</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>score</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>match_result_values</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>destTable</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>sourceTable</t>
+          <t>nombre_completo</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>77.19298245614034%</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Downs</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>user1@example.com</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>DavidDownsuser1@example.com</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>DeborahDavisuser21@example.com</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>77.19298245614034</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>{'nombre': 'Deborah', 'apellido': 'Davis', 'email': 'user21@example.com'}</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Clientes</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Usuarios</t>
+          <t>David Downs</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>82.75862068965517%</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Davis</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>user2@example.com</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>RobertDavisuser2@example.com</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>DeborahDavisuser21@example.com</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>82.75862068965517</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>{'nombre': 'Deborah', 'apellido': 'Davis', 'email': 'user21@example.com'}</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Clientes</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Usuarios</t>
+          <t>Robert Davis</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mary</t>
+          <t>80.0%</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Wells</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>user3@example.com</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>MaryWellsuser3@example.com</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>MaryPollarduser12@example.com</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>80</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>{'nombre': 'Mary', 'apellido': 'Pollard', 'email': 'user12@example.com'}</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Clientes</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Usuarios</t>
+          <t>Mary Wells</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bethany</t>
+          <t>77.41935483870968%</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Harmon</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>user4@example.com</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>BethanyHarmonuser4@example.com</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>DanielHarrisonuser48@example.com</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>77.41935483870968</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>{'nombre': 'Daniel', 'apellido': 'Harrison', 'email': 'user48@example.com'}</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Clientes</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Usuarios</t>
+          <t>Bethany Harmon</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>81.9672131147541%</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Brenda Meyers</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>75.0%</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Yvonne Jensen</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>75.86206896551724%</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Joe Ferguson</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>April Gonzalez</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Colton Collins</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Joseph Yang</t>
         </is>
       </c>
     </row>

</xml_diff>